<commit_message>
Made a new BOM for V4
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V4.xlsx
+++ b/BOM/BOM_PowerBoard_V4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E325706C-087F-8C4C-964E-60C4E5FAAF23}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470F251A-5645-7E4B-B5EA-5BFFE2DADDD6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="640" windowWidth="23680" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
@@ -445,10 +445,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +768,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="A11:G11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added stuff to V4
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V4.xlsx
+++ b/BOM/BOM_PowerBoard_V4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470F251A-5645-7E4B-B5EA-5BFFE2DADDD6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D750DAE9-21F0-1240-98DB-2F5D8DBE3D3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="640" windowWidth="23680" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="23680" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +788,7 @@
       </c>
       <c r="B1" s="15">
         <f>SUM(G3:G193)</f>
-        <v>176.16000000000003</v>
+        <v>176.62000000000003</v>
       </c>
       <c r="D1" t="s">
         <v>78</v>
@@ -986,14 +986,14 @@
         <v>11</v>
       </c>
       <c r="E9" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="9">
         <v>0.46</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="0"/>
-        <v>1.3800000000000001</v>
+        <v>1.84</v>
       </c>
       <c r="H9" s="6"/>
       <c r="J9" s="2"/>

</xml_diff>

<commit_message>
added 5V 4A DC/DC Power Supply to BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V4.xlsx
+++ b/BOM/BOM_PowerBoard_V4.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCC\GitHub\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D750DAE9-21F0-1240-98DB-2F5D8DBE3D3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764CAD49-6A92-407C-87AE-9A6A64520438}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="23680" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="1920" yWindow="456" windowWidth="23676" windowHeight="15540" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t xml:space="preserve">14-32V to 12V 2A DC-DC Converter </t>
+  </si>
+  <si>
+    <t>R-745.0P</t>
+  </si>
+  <si>
+    <t>5V 4A Output Power Supply</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -451,6 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,34 +774,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DE3487-35ED-9947-B91A-5715036B4C63}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" customWidth="1"/>
+    <col min="4" max="4" width="38.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="15">
         <f>SUM(G3:G193)</f>
-        <v>176.62000000000003</v>
+        <v>212.31000000000006</v>
       </c>
       <c r="D1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -820,7 +827,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>51</v>
       </c>
@@ -845,7 +852,7 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>53</v>
       </c>
@@ -870,7 +877,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>75</v>
       </c>
@@ -896,7 +903,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="14" t="s">
         <v>48</v>
@@ -919,7 +926,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>55</v>
       </c>
@@ -944,7 +951,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -972,7 +979,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
@@ -1030,21 +1037,36 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>35.69</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>35.69</v>
+      </c>
+      <c r="H11" s="22"/>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>56</v>
       </c>
@@ -1073,7 +1095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="14" t="s">
         <v>16</v>
@@ -1096,7 +1118,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>1845344</v>
       </c>
@@ -1121,7 +1143,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1715721</v>
       </c>
@@ -1146,7 +1168,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1715190</v>
       </c>
@@ -1171,7 +1193,7 @@
       </c>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>1988998</v>
       </c>
@@ -1196,7 +1218,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>63</v>
       </c>
@@ -1221,7 +1243,7 @@
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
@@ -1246,7 +1268,7 @@
       </c>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
@@ -1271,7 +1293,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>86</v>
       </c>
@@ -1296,7 +1318,7 @@
       </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -1321,7 +1343,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>38</v>
       </c>
@@ -1346,7 +1368,7 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>41</v>
       </c>
@@ -1371,7 +1393,7 @@
       </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>42</v>
       </c>
@@ -1396,7 +1418,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>44</v>
       </c>
@@ -1421,7 +1443,7 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>45</v>
       </c>
@@ -1446,7 +1468,7 @@
       </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>26</v>
       </c>
@@ -1471,7 +1493,7 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>28</v>
       </c>
@@ -1496,7 +1518,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>59</v>
       </c>
@@ -1521,7 +1543,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>49</v>
       </c>
@@ -1546,7 +1568,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>744772390</v>
       </c>
@@ -1571,7 +1593,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>35</v>
       </c>
@@ -1596,7 +1618,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>79</v>
       </c>
@@ -1621,7 +1643,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Did some more stuff
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V4.xlsx
+++ b/BOM/BOM_PowerBoard_V4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85362BB-2F3A-0A4A-A9B4-BCF26F13FE9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD744580-4C84-EA41-8239-6E6EF1B276D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="460" windowWidth="33400" windowHeight="23100" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
+    <workbookView xWindow="2020" yWindow="1660" windowWidth="22520" windowHeight="22820" xr2:uid="{067DA466-7928-7D4E-AB9E-6DB7CCDA03D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,6 @@
     <t>50V 10uF Capacitor</t>
   </si>
   <si>
-    <t>EEE-FK1E101SP</t>
-  </si>
-  <si>
-    <t>25V 100uF Capacitor</t>
-  </si>
-  <si>
     <t>EEE-FK1V680SP</t>
   </si>
   <si>
@@ -316,6 +310,12 @@
   </si>
   <si>
     <t>RES SMD 2K OHM 0.5% 1/16W 0603</t>
+  </si>
+  <si>
+    <t>EEE-1HA101UP</t>
+  </si>
+  <si>
+    <t>CAP ALUM 100UF 20% 50V SMD 0.315" Dia (8.00mm)</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -482,6 +482,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -813,7 +814,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,14 +830,14 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15">
         <f>SUM(G3:G191)</f>
-        <v>258.72000000000008</v>
+        <v>259.22000000000008</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -859,15 +860,15 @@
         <v>3</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>4</v>
@@ -876,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="9">
         <v>2</v>
@@ -892,7 +893,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>4</v>
@@ -901,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="9">
         <v>13</v>
@@ -917,16 +918,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="E5" s="9">
         <v>3</v>
@@ -944,13 +945,13 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="9">
         <v>2</v>
@@ -966,7 +967,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>9</v>
@@ -990,8 +991,8 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>12</v>
+      <c r="A8" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>9</v>
@@ -999,22 +1000,22 @@
       <c r="C8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="9">
-        <v>3</v>
+      <c r="D8" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="25">
+        <v>4</v>
       </c>
       <c r="F8" s="9">
         <v>0.5</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H8" s="6"/>
       <c r="J8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1043,12 +1044,12 @@
       <c r="H9" s="6"/>
       <c r="J9" s="2"/>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>9</v>
@@ -1057,7 +1058,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="9">
         <v>1</v>
@@ -1072,21 +1073,21 @@
       <c r="H10" s="6"/>
       <c r="J10" s="7"/>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="E11" s="9">
         <v>1</v>
@@ -1101,21 +1102,21 @@
       <c r="H11" s="20"/>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="9">
         <v>3</v>
@@ -1130,21 +1131,21 @@
       <c r="H12" s="6"/>
       <c r="J12" s="4"/>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="24">
+        <v>61</v>
+      </c>
+      <c r="E13" s="25">
         <v>2</v>
       </c>
       <c r="F13" s="9">
@@ -1155,9 +1156,9 @@
         <v>17.36</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="J13" s="21"/>
+      <c r="J13" s="22"/>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1165,13 +1166,13 @@
         <v>1715190</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="9">
         <v>4</v>
@@ -1190,13 +1191,13 @@
         <v>1988998</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="9">
         <v>2</v>
@@ -1212,16 +1213,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -1237,16 +1238,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
@@ -1261,45 +1262,45 @@
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="23">
+        <v>35.69</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="22">
-        <v>35.69</v>
-      </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="25">
+      <c r="B19" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="26">
         <v>1</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="23">
         <v>78.53</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="26">
         <f t="shared" ref="G19" si="2">F19*E19</f>
         <v>78.53</v>
       </c>
@@ -1307,16 +1308,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="C20" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
@@ -1332,16 +1333,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="E21" s="9">
         <v>2</v>
@@ -1357,7 +1358,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>9</v>
@@ -1366,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>
@@ -1382,7 +1383,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>9</v>
@@ -1391,7 +1392,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -1407,7 +1408,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>9</v>
@@ -1416,7 +1417,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="9">
         <v>1</v>
@@ -1432,7 +1433,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>9</v>
@@ -1441,7 +1442,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E25" s="9">
         <v>1</v>
@@ -1457,7 +1458,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>9</v>
@@ -1466,7 +1467,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" s="9">
         <v>10</v>
@@ -1482,7 +1483,7 @@
     </row>
     <row r="27" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>9</v>
@@ -1491,7 +1492,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E27" s="9">
         <v>4</v>
@@ -1507,16 +1508,16 @@
     </row>
     <row r="28" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E28" s="9">
         <v>1</v>
@@ -1532,7 +1533,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>9</v>
@@ -1541,7 +1542,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E29" s="9">
         <v>2</v>
@@ -1560,13 +1561,13 @@
         <v>744772390</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E30" s="9">
         <v>1</v>
@@ -1582,16 +1583,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E31" s="9">
         <v>2</v>
@@ -1607,16 +1608,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" s="9">
         <v>1</v>
@@ -1632,18 +1633,18 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="24">
+      <c r="E33" s="25">
         <v>2</v>
       </c>
       <c r="F33" s="11">
@@ -1656,111 +1657,111 @@
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="22">
+      <c r="A34" s="23">
         <v>74479776247</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="22" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="25">
+        <v>1</v>
+      </c>
+      <c r="F34" s="23">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G34" s="25">
+        <f t="shared" si="1"/>
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E35" s="23">
         <v>1</v>
       </c>
-      <c r="F34" s="22">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G34" s="24">
-        <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
+      <c r="F35" s="23">
+        <v>1.87</v>
+      </c>
+      <c r="G35" s="25">
+        <f t="shared" si="1"/>
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="25">
+        <v>1</v>
+      </c>
+      <c r="F36" s="23">
+        <v>1.74</v>
+      </c>
+      <c r="G36" s="25">
+        <f t="shared" si="1"/>
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="23">
+        <v>395311002</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="22">
-        <v>1</v>
-      </c>
-      <c r="F35" s="22">
-        <v>1.87</v>
-      </c>
-      <c r="G35" s="24">
-        <f t="shared" si="1"/>
-        <v>1.87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="24">
-        <v>1</v>
-      </c>
-      <c r="F36" s="22">
-        <v>1.74</v>
-      </c>
-      <c r="G36" s="24">
-        <f t="shared" si="1"/>
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="22">
-        <v>395311002</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="22" t="s">
+      <c r="E37" s="25">
+        <v>6</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.51</v>
+      </c>
+      <c r="G37" s="25">
+        <f t="shared" si="1"/>
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="24">
-        <v>6</v>
-      </c>
-      <c r="F37" s="22">
-        <v>0.51</v>
-      </c>
-      <c r="G37" s="24">
-        <f t="shared" si="1"/>
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="24">
+      <c r="B38" s="22"/>
+      <c r="C38" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="25">
         <v>2</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="23">
         <v>0.11</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="25">
         <f t="shared" si="1"/>
         <v>0.22</v>
       </c>

</xml_diff>

<commit_message>
Updated BOM to include new 3A Inductor for 60W 12V power supply
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V4.xlsx
+++ b/BOM/BOM_PowerBoard_V4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
   <si>
     <t xml:space="preserve">Total Cost</t>
   </si>
@@ -289,7 +289,10 @@
     <t xml:space="preserve">Mosfet P-Channel 30V 3.8A SOT-23-3</t>
   </si>
   <si>
-    <t xml:space="preserve">FIXED IND 4.7UH 1A 160 MOHM SMD 0806 (2016 Metric)</t>
+    <t xml:space="preserve">LHL08TB4R7M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXED IND 4.7UH 3A 25 MOHM TH</t>
   </si>
   <si>
     <t xml:space="preserve">CGA6P3X7S1H685M250AB</t>
@@ -322,7 +325,7 @@
     <t xml:space="preserve">Digikey Cart (07/23):</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.ca/short/j5d973</t>
+    <t xml:space="preserve">https://www.digikey.ca/short/j5v9jw</t>
   </si>
   <si>
     <t xml:space="preserve">Arrow pg for 395300002:</t>
@@ -338,7 +341,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -402,12 +405,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -576,7 +573,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -584,7 +581,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -683,22 +680,22 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.7851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.7666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,14 +704,21 @@
       </c>
       <c r="B1" s="4" t="n">
         <f aca="false">SUM(G3:G191)</f>
-        <v>225.37</v>
-      </c>
+        <v>224.68</v>
+      </c>
+      <c r="C1" s="0"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -741,6 +745,9 @@
       <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
@@ -765,6 +772,10 @@
         <f aca="false">E3*F3</f>
         <v>4.48</v>
       </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
@@ -789,6 +800,10 @@
         <f aca="false">E4*F4</f>
         <v>18.85</v>
       </c>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
@@ -813,7 +828,10 @@
         <f aca="false">E5*F5</f>
         <v>1.02</v>
       </c>
+      <c r="H5" s="0"/>
       <c r="I5" s="2"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
@@ -838,6 +856,9 @@
         <f aca="false">E6*F6</f>
         <v>0.38</v>
       </c>
+      <c r="H6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
@@ -847,6 +868,9 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
+      <c r="H7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
@@ -871,9 +895,11 @@
         <f aca="false">E8*F8</f>
         <v>3.8</v>
       </c>
+      <c r="H8" s="0"/>
       <c r="J8" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="K8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
@@ -898,6 +924,7 @@
         <f aca="false">E9*F9</f>
         <v>2.8</v>
       </c>
+      <c r="H9" s="0"/>
       <c r="J9" s="13"/>
       <c r="K9" s="1" t="s">
         <v>30</v>
@@ -926,6 +953,7 @@
         <f aca="false">E10*F10</f>
         <v>0.8</v>
       </c>
+      <c r="H10" s="0"/>
       <c r="J10" s="14"/>
       <c r="K10" s="1" t="s">
         <v>33</v>
@@ -939,6 +967,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
+      <c r="H11" s="0"/>
       <c r="J11" s="15"/>
       <c r="K11" s="1" t="s">
         <v>34</v>
@@ -967,6 +996,7 @@
         <f aca="false">E12*F12</f>
         <v>1.98</v>
       </c>
+      <c r="H12" s="0"/>
       <c r="J12" s="16"/>
       <c r="K12" s="1" t="s">
         <v>38</v>
@@ -1479,37 +1509,39 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21" t="n">
-        <v>74479776247</v>
-      </c>
-      <c r="B34" s="18"/>
+      <c r="A34" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="C34" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E34" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F34" s="21" t="n">
-        <v>1.15</v>
+        <v>0.46</v>
       </c>
       <c r="G34" s="11" t="n">
         <f aca="false">E34*F34</f>
-        <v>1.15</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E35" s="21" t="n">
         <v>1</v>
@@ -1524,14 +1556,14 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E36" s="11" t="n">
         <v>1</v>
@@ -1553,7 +1585,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E37" s="11" t="n">
         <v>6</v>
@@ -1571,13 +1603,13 @@
         <v>395300002</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>6</v>
@@ -1592,14 +1624,14 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E39" s="11" t="n">
         <v>2</v>
@@ -1612,26 +1644,27 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B41" r:id="rId1" display="https://www.digikey.ca/short/j5d973"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>